<commit_message>
Fix addFonted and createNewSheet
</commit_message>
<xml_diff>
--- a/2024_2025_AM1_AM2_AM3_PoiGanttSkeleton/src/test/resources/output/EggsScrambled.xlsx
+++ b/2024_2025_AM1_AM2_AM3_PoiGanttSkeleton/src/test/resources/output/EggsScrambled.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Tasks" r:id="rId3" sheetId="1"/>
+    <sheet name="File too" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="23">
   <si>
     <t xml:space="preserve">      </t>
   </si>
@@ -78,6 +79,9 @@
   </si>
   <si>
     <t>Wash fry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -85,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -93,13 +97,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,8 +131,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left" wrapText="false"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -128,12 +148,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="4.5234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.54296875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.5234375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="35.203125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="5.05859375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="5.890625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="4.0234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="5.6484375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.3828125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="35.1875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.96875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.1171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -586,4 +606,216 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:Z4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="4.78515625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.37890625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.3828125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="5.640625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.375" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="n" s="0">
+        <v>100.0</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>91.0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="n" s="0">
+        <v>200.0</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>56.0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="n" s="0">
+        <v>300.0</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>149.0</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more Fonts to CreateNewSheet
</commit_message>
<xml_diff>
--- a/2024_2025_AM1_AM2_AM3_PoiGanttSkeleton/src/test/resources/output/EggsScrambled.xlsx
+++ b/2024_2025_AM1_AM2_AM3_PoiGanttSkeleton/src/test/resources/output/EggsScrambled.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="23">
   <si>
     <t xml:space="preserve">      </t>
   </si>
@@ -610,7 +610,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -618,8 +618,8 @@
   <cols>
     <col min="1" max="1" width="4.78515625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="6.37890625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="4.3828125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="17.31640625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="4.7890625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="37.65234375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="5.640625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="6.375" customWidth="true" bestFit="true"/>
   </cols>
@@ -705,16 +705,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="C2" t="n" s="0">
+      <c r="B2" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2" t="n" s="1">
         <v>100.0</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="E2" t="n" s="0">
+      <c r="E2" t="n" s="1">
         <v>60.0</v>
       </c>
-      <c r="F2" t="n" s="0">
+      <c r="F2" t="n" s="1">
         <v>91.0</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -755,63 +758,316 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" t="n" s="0">
+      <c r="C3" t="n" s="1">
+        <v>101.0</v>
+      </c>
+      <c r="D3" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="E3" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F3" t="n" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="n" s="1">
+        <v>102.0</v>
+      </c>
+      <c r="D4" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F4" t="n" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="n" s="1">
+        <v>103.0</v>
+      </c>
+      <c r="D5" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="E5" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F5" t="n" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="n" s="1">
+        <v>105.0</v>
+      </c>
+      <c r="D6" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="E6" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F6" t="n" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="n" s="1">
+        <v>104.0</v>
+      </c>
+      <c r="D7" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="E7" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F7" t="n" s="1">
+        <v>17.0</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="n" s="1">
+        <v>106.0</v>
+      </c>
+      <c r="D8" t="s" s="1">
+        <v>14</v>
+      </c>
+      <c r="E8" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F8" t="n" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n" s="1">
         <v>200.0</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D9" t="s" s="1">
         <v>15</v>
       </c>
-      <c r="E3" t="n" s="0">
+      <c r="E9" t="n" s="1">
         <v>20.0</v>
       </c>
-      <c r="F3" t="n" s="0">
+      <c r="F9" t="n" s="1">
         <v>56.0</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="n" s="0">
+      <c r="P9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="C10" t="n" s="1">
+        <v>201.0</v>
+      </c>
+      <c r="D10" t="s" s="1">
+        <v>16</v>
+      </c>
+      <c r="E10" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F10" t="n" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="n" s="1">
+        <v>202.0</v>
+      </c>
+      <c r="D11" t="s" s="1">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F11" t="n" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="1">
+        <v>6</v>
+      </c>
+      <c r="C12" t="n" s="1">
         <v>300.0</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D12" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="E4" t="n" s="0">
+      <c r="E12" t="n" s="1">
         <v>30.0</v>
       </c>
-      <c r="F4" t="n" s="0">
+      <c r="F12" t="n" s="1">
         <v>149.0</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z4" s="1" t="s">
+      <c r="S12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="C13" t="n" s="1">
+        <v>301.0</v>
+      </c>
+      <c r="D13" t="s" s="1">
+        <v>19</v>
+      </c>
+      <c r="E13" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F13" t="n" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="n" s="1">
+        <v>302.0</v>
+      </c>
+      <c r="D14" t="s" s="1">
+        <v>20</v>
+      </c>
+      <c r="E14" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F14" t="n" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="n" s="1">
+        <v>303.0</v>
+      </c>
+      <c r="D15" t="s" s="1">
+        <v>21</v>
+      </c>
+      <c r="E15" t="n" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="F15" t="n" s="1">
+        <v>49.0</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z15" s="1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>